<commit_message>
Code updated 23-03-30 13:58:00
</commit_message>
<xml_diff>
--- a/Season_Trophies/87.xlsx
+++ b/Season_Trophies/87.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E124"/>
+  <dimension ref="A1:E127"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -396,7 +396,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>56496</t>
+          <t>56650</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -423,17 +423,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2917</t>
+          <t>1124</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>27468237</t>
+          <t>6940556</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>佛系复仇者秀川</t>
+          <t>"Cry ab it林黛玉ᶻᵍˣ"</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -443,24 +443,24 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>4454</t>
+          <t>4618</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>9765</t>
+          <t>1344</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>14424176</t>
+          <t>20199374</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>天才少年老纪</t>
+          <t>RuanFan</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -470,24 +470,24 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>4125</t>
+          <t>4591</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>15473</t>
+          <t>493</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>43800641</t>
+          <t>8741713</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>㊥蛋蛋大</t>
+          <t xml:space="preserve">㊥大咖玩家ky </t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -497,24 +497,24 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>3981</t>
+          <t>4728</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>20415</t>
+          <t>1297</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>4229136</t>
+          <t>46422609</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>"totoro wu"</t>
+          <t>㊥林天大大神</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -524,24 +524,24 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>3811</t>
+          <t>4596</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>49108</t>
+          <t>2967</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>21665473</t>
+          <t>1951758</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>"Dog Gamedesiger"</t>
+          <t>我來找你了</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -551,24 +551,24 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2746</t>
+          <t>4459</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>1275</t>
+          <t>3036</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>20199374</t>
+          <t>27468237</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>RuanFan</t>
+          <t>佛系复仇者秀川</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -578,24 +578,24 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>4591</t>
+          <t>4454</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2849</t>
+          <t>9557</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>1951758</t>
+          <t>14424176</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>我來找你了</t>
+          <t>天才少年老纪</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -605,24 +605,24 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>4459</t>
+          <t>4146</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>7840</t>
+          <t>16001</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>25376635</t>
+          <t>43800641</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>"sanchez ᶻᵍˣ"</t>
+          <t>㊥蛋蛋大</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -632,24 +632,24 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>4206</t>
+          <t>3981</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>24978</t>
+          <t>16774</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>45967307</t>
+          <t>26588375</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Ricky</t>
+          <t>何苦僧ai</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -659,24 +659,24 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>3660</t>
+          <t>3958</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>25739</t>
+          <t>21076</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>12333251</t>
+          <t>4229136</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>"㊌ Mingxuan"</t>
+          <t>"totoro wu"</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -686,24 +686,24 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>3635</t>
+          <t>3811</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>39343</t>
+          <t>49289</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>37069173</t>
+          <t>21665473</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>詹toniii</t>
+          <t>"Dog Gamedesiger"</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -713,24 +713,24 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>3117</t>
+          <t>2746</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>40877</t>
+          <t>8116</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>55634661</t>
+          <t>25376635</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Opalus</t>
+          <t>"sanchez ᶻᵍˣ"</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -740,24 +740,24 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>3043</t>
+          <t>4206</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>46001</t>
+          <t>25646</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>20737010</t>
+          <t>45967307</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>混着玩...</t>
+          <t>Ricky</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -767,24 +767,24 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2843</t>
+          <t>3660</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>55703</t>
+          <t>25946</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>59095922</t>
+          <t>12333251</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>xxxx7</t>
+          <t>"㊌ Mingxuan"</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -794,24 +794,24 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2592</t>
+          <t>3650</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>58833</t>
+          <t>39667</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>37069173</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>春田花花幼稚园</t>
+          <t>詹toniii</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -821,24 +821,24 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2547</t>
+          <t>3115</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>60989</t>
+          <t>41103</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>7587898</t>
+          <t>55634661</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>藍精靈ᶻᵍˣ</t>
+          <t>Opalus</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -848,24 +848,24 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2521</t>
+          <t>3043</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>61518</t>
+          <t>46176</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>6510348</t>
+          <t>20737010</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Bonpoisson</t>
+          <t>混着玩...</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -875,24 +875,24 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2516</t>
+          <t>2843</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>68483</t>
+          <t>55865</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>59093405</t>
+          <t>59095922</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>永恒不朽6</t>
+          <t>xxxx7</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -902,24 +902,24 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>2269</t>
+          <t>2592</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>84567</t>
+          <t>58981</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>59100545</t>
+          <t>20</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>"black dragon"</t>
+          <t>春田花花幼稚园</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -929,24 +929,24 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>1719</t>
+          <t>2547</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>61106</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>23687250</t>
+          <t>7587898</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>"jetlijp ᶻᵍˣ"</t>
+          <t>藍精靈ᶻᵍˣ</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -956,24 +956,24 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2521</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>61631</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>47928278</t>
+          <t>6510348</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>"落日幻影 哈哈哈"</t>
+          <t>Bonpoisson</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -983,24 +983,24 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2516</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>1164</t>
+          <t>68588</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>46422609</t>
+          <t>59093405</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>㊥林天大大神</t>
+          <t>永恒不朽6</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1010,105 +1010,105 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>4605</t>
+          <t>2269</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>22921</t>
+          <t>84716</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>37861953</t>
+          <t>59100545</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>"Durex ๑• . •๑"</t>
+          <t>"black dragon"</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>3729</t>
+          <t>1719</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>8341</t>
+          <t>999999</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>31217211</t>
+          <t>23687250</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>解憂雜貨鋪㊥</t>
+          <t>"jetlijp ᶻᵍˣ"</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>4184</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>11244</t>
+          <t>999999</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>53520939</t>
+          <t>47928278</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>㊥虎哥tiger</t>
+          <t>"落日幻影 哈哈哈"</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>4065</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>21422</t>
+          <t>23588</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>38809086</t>
+          <t>37861953</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Kouenᶻᵍˣ</t>
+          <t>"Durex ๑• . •๑"</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1118,24 +1118,24 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>3778</t>
+          <t>3729</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>26635</t>
+          <t>8611</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>47146736</t>
+          <t>31217211</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>"HK 品瑜"</t>
+          <t>解憂雜貨鋪㊥</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1145,24 +1145,24 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>3607</t>
+          <t>4184</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>8720</t>
+          <t>11806</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>53060417</t>
+          <t>53520939</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>㊥老纳信耶稣</t>
+          <t>㊥虎哥tiger</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1172,24 +1172,24 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>4168</t>
+          <t>4060</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>12223</t>
+          <t>22092</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>49710892</t>
+          <t>38809086</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>MMMMMMM</t>
+          <t>Kouenᶻᵍˣ</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1199,24 +1199,24 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>4030</t>
+          <t>3778</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>12780</t>
+          <t>27360</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>54698813</t>
+          <t>47146736</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>閃亮唐老鴨</t>
+          <t>"HK 品瑜"</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1226,24 +1226,24 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>4013</t>
+          <t>3605</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>13619</t>
+          <t>5134</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>31495601</t>
+          <t>49710892</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>陈晓军</t>
+          <t>MMMMMMM</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1253,24 +1253,24 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>3997</t>
+          <t>4343</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>14531</t>
+          <t>9484</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>4756174</t>
+          <t>53060417</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>純希です</t>
+          <t>㊥老纳信耶稣</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1280,24 +1280,24 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>3991</t>
+          <t>4148</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>15318</t>
+          <t>13763</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>8057001</t>
+          <t>54698813</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>㊥兵者诡道也</t>
+          <t>閃亮唐老鴨</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1307,24 +1307,24 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>3983</t>
+          <t>4003</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>34672</t>
+          <t>14226</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>55769051</t>
+          <t>31495601</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>㊥叮叮当.</t>
+          <t>陈晓军</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1334,24 +1334,24 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>3320</t>
+          <t>3997</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>4638</t>
+          <t>15270</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>4493731</t>
+          <t>4756174</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Player-1527362</t>
+          <t>純希です</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1361,24 +1361,24 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>4359</t>
+          <t>3990</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>6407</t>
+          <t>15852</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>47131129</t>
+          <t>8057001</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>NAM</t>
+          <t>㊥兵者诡道也</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1388,24 +1388,24 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>4276</t>
+          <t>3983</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>8661</t>
+          <t>35075</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>24733875</t>
+          <t>55769051</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>龍少</t>
+          <t>㊥叮叮当.</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1415,24 +1415,24 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>4171</t>
+          <t>3319</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>10391</t>
+          <t>4818</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>7852598</t>
+          <t>4493731</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>seiji</t>
+          <t>Player-1527362</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1442,24 +1442,24 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>4097</t>
+          <t>4359</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>11121</t>
+          <t>6603</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>46289694</t>
+          <t>47131129</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>㊥Vincent</t>
+          <t>NAM</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1469,24 +1469,24 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>4069</t>
+          <t>4276</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>10226</t>
+          <t>7997</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>38995116</t>
+          <t>55317038</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>"Ramesh Pavai Nam"</t>
+          <t>necman12345</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -1496,24 +1496,24 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>4104</t>
+          <t>4210</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>12498</t>
+          <t>8943</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>56133764</t>
+          <t>24733875</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>ustcarter</t>
+          <t>龍少</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -1523,24 +1523,24 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>4021</t>
+          <t>4171</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>14357</t>
+          <t>10012</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>54085771</t>
+          <t>38995116</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>㊥Matthieu</t>
+          <t>"Ramesh Pavai Nam"</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -1550,24 +1550,24 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>3992</t>
+          <t>4128</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>15086</t>
+          <t>10779</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>55317038</t>
+          <t>7852598</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>necman12345</t>
+          <t>seiji</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -1577,24 +1577,24 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>3986</t>
+          <t>4097</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>16343</t>
+          <t>12539</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>54778421</t>
+          <t>46289694</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Emma</t>
+          <t>㊥Vincent</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1604,24 +1604,24 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>3954</t>
+          <t>4036</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>19585</t>
+          <t>13523</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>11582001</t>
+          <t>56133764</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>iMinatoX4</t>
+          <t>ustcarter</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -1631,24 +1631,24 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>3839</t>
+          <t>4008</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>21425</t>
+          <t>13821</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>31401481</t>
+          <t>54085771</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Player-31401481</t>
+          <t>㊥Matthieu</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -1658,24 +1658,24 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>3778</t>
+          <t>4002</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>24388</t>
+          <t>16532</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>56732705</t>
+          <t>54778421</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>时间温柔皆遗憾</t>
+          <t>Emma</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -1685,24 +1685,24 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>3680</t>
+          <t>3966</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>24729</t>
+          <t>20186</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>56585361</t>
+          <t>11582001</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>"㊥ go策划我要ali"</t>
+          <t>iMinatoX4</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -1712,24 +1712,24 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>3668</t>
+          <t>3839</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>24702</t>
+          <t>22173</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>58839983</t>
+          <t>31401481</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>每逢佳节胖六斤</t>
+          <t>Player-31401481</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -1739,24 +1739,24 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>3669</t>
+          <t>3775</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>25232</t>
+          <t>24444</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>6809364</t>
+          <t>56732705</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>"Scorp IP"</t>
+          <t>时间温柔皆遗憾</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -1766,24 +1766,24 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>3651</t>
+          <t>3701</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>28192</t>
+          <t>25662</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>56379103</t>
+          <t>58839983</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Globalking1001</t>
+          <t>每逢佳节胖六斤</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -1793,24 +1793,24 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>3554</t>
+          <t>3659</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>29565</t>
+          <t>25719</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>47459684</t>
+          <t>56585361</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>㊥阿闹切克闹</t>
+          <t>"㊥ go策划我要ali"</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -1820,24 +1820,24 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>3508</t>
+          <t>3657</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>29582</t>
+          <t>25885</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>58408326</t>
+          <t>6809364</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>"Killer Bee"</t>
+          <t>"Scorp IP"</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -1847,24 +1847,24 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>3507</t>
+          <t>3651</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>33201</t>
+          <t>25932</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>50837459</t>
+          <t>56379103</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>NINE日</t>
+          <t>Globalking1001</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -1874,24 +1874,24 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>3376</t>
+          <t>3650</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>34918</t>
+          <t>27528</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>56573048</t>
+          <t>58408326</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Xiaotian</t>
+          <t>"Killer Bee"</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -1901,24 +1901,24 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>3310</t>
+          <t>3599</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>36392</t>
+          <t>29567</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>57813281</t>
+          <t>47459684</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>XAUEN</t>
+          <t>㊥阿闹切克闹</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -1928,24 +1928,24 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>3249</t>
+          <t>3529</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>36869</t>
+          <t>31257</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>58203298</t>
+          <t>3649043</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>权旨qua</t>
+          <t>Dj6106</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -1955,24 +1955,24 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>3230</t>
+          <t>3468</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>37370</t>
+          <t>33681</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>1304123</t>
+          <t>50837459</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Cccccccccccc</t>
+          <t>NINE日</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -1982,24 +1982,24 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>3209</t>
+          <t>3375</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>38948</t>
+          <t>35337</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>56500325</t>
+          <t>56573048</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>haruharuyukizg9735</t>
+          <t>Xiaotian</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -2009,24 +2009,24 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>3135</t>
+          <t>3308</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>39561</t>
+          <t>36741</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>3649043</t>
+          <t>57813281</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Dj6106</t>
+          <t>XAUEN</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -2036,24 +2036,24 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>3104</t>
+          <t>3249</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>40090</t>
+          <t>36388</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>38561634</t>
+          <t>58203298</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>"Ambrose PT"</t>
+          <t>权旨qua</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -2063,24 +2063,24 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>3079</t>
+          <t>3264</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>42697</t>
+          <t>37499</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>52997727</t>
+          <t>1304123</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>larios</t>
+          <t>Cccccccccccc</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -2090,24 +2090,24 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>2965</t>
+          <t>3218</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>45160</t>
+          <t>39342</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>48634530</t>
+          <t>56500325</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>leezhenrui</t>
+          <t>haruharuyukizg9735</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -2117,24 +2117,24 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>2870</t>
+          <t>3131</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>45993</t>
+          <t>40421</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>32316256</t>
+          <t>38561634</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>"秋の風 .."</t>
+          <t>"Ambrose PT"</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -2144,24 +2144,24 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>2843</t>
+          <t>3077</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>46861</t>
+          <t>42912</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>55860890</t>
+          <t>52997727</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>㊥Ethan</t>
+          <t>larios</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -2171,24 +2171,24 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>2815</t>
+          <t>2965</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>54567</t>
+          <t>44909</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>38893233</t>
+          <t>48634530</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>"快乐 二哈"</t>
+          <t>leezhenrui</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -2198,24 +2198,24 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>2614</t>
+          <t>2886</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>60074</t>
+          <t>46171</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>1550355</t>
+          <t>32316256</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>"皓茵 世界"</t>
+          <t>"秋の風 .."</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -2225,105 +2225,105 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>2532</t>
+          <t>2843</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>11805</t>
+          <t>47067</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>31134300</t>
+          <t>55860890</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>McMaX</t>
+          <t>㊥Ethan</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>4045</t>
+          <t>2814</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>54163</t>
+          <t>54729</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>43281368</t>
+          <t>38893233</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>xhs2763</t>
+          <t>"快乐 二哈"</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>2622</t>
+          <t>2614</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>63179</t>
+          <t>60195</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>44378757</t>
+          <t>1550355</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>"NᵉᵗʰᵉʳDʳⁱᶠᵗᵉʳ ㊥"</t>
+          <t>"皓茵 世界"</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>2500</t>
+          <t>2532</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>12271</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>48738257</t>
+          <t>31134300</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>死亡洲际跳蛋</t>
+          <t>McMaX</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -2333,24 +2333,24 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>4045</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>22707</t>
+          <t>54332</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>44708798</t>
+          <t>43281368</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>"㊥ mythgod"</t>
+          <t>xhs2763</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -2360,24 +2360,24 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>3736</t>
+          <t>2622</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>27520</t>
+          <t>63259</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>25479797</t>
+          <t>44378757</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>"Mohamed Alnaqbi"</t>
+          <t>"NᵉᵗʰᵉʳDʳⁱᶠᵗᵉʳ ㊥"</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -2387,24 +2387,24 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>3577</t>
+          <t>2500</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>44379</t>
+          <t>999999</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>54588689</t>
+          <t>48738257</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>㊥墨衍枫迹☜</t>
+          <t>死亡洲际跳蛋</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -2414,24 +2414,24 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>2897</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>56760</t>
+          <t>22433</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>28855852</t>
+          <t>44708798</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>tiger</t>
+          <t>"㊥ mythgod"</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -2441,24 +2441,24 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>2576</t>
+          <t>3766</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>29815</t>
+          <t>28170</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>18082891</t>
+          <t>25479797</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Michael</t>
+          <t>"Mohamed Alnaqbi"</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -2468,24 +2468,24 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>3499</t>
+          <t>3577</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>34919</t>
+          <t>44597</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>55499394</t>
+          <t>54588689</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Player-55499394</t>
+          <t>㊥墨衍枫迹☜</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -2495,24 +2495,24 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>3310</t>
+          <t>2897</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>44788</t>
+          <t>56985</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>56700848</t>
+          <t>28855852</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>工口漫画老师</t>
+          <t>tiger</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -2522,24 +2522,24 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>2883</t>
+          <t>2575</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>47448</t>
+          <t>26467</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>9718882</t>
+          <t>18082891</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>小霸王2021</t>
+          <t>Michael</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -2549,24 +2549,24 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>2796</t>
+          <t>3632</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>58594</t>
+          <t>27314</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>47430231</t>
+          <t>55499394</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Kentantrino</t>
+          <t>Player-55499394</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -2576,24 +2576,24 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>2550</t>
+          <t>3606</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>59326</t>
+          <t>44989</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>11645391</t>
+          <t>56700848</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>"omar omar"</t>
+          <t>工口漫画老师</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
@@ -2603,24 +2603,24 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>2541</t>
+          <t>2883</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>60383</t>
+          <t>47628</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>52792063</t>
+          <t>9718882</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>"Tramaine Dowlen"</t>
+          <t>小霸王2021</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -2630,24 +2630,24 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>2528</t>
+          <t>2796</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>62000</t>
+          <t>58811</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>3391765</t>
+          <t>47430231</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>马er</t>
+          <t>Kentantrino</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
@@ -2657,24 +2657,24 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>2512</t>
+          <t>2549</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>63945</t>
+          <t>59478</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>5367482</t>
+          <t>11645391</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Ігор</t>
+          <t>"omar omar"</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
@@ -2684,24 +2684,24 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>2497</t>
+          <t>2541</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>65569</t>
+          <t>60594</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>15436348</t>
+          <t>52792063</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Lucas</t>
+          <t>"Tramaine Dowlen"</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
@@ -2711,24 +2711,24 @@
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>2484</t>
+          <t>2527</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>89666</t>
+          <t>62110</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>54941706</t>
+          <t>3391765</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>AlexMenjivar20</t>
+          <t>马er</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
@@ -2738,24 +2738,24 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>1550</t>
+          <t>2512</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>94769</t>
+          <t>64013</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>57219176</t>
+          <t>5367482</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>青莲道人</t>
+          <t>Ігор</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
@@ -2765,24 +2765,24 @@
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>1500</t>
+          <t>2497</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>112804</t>
+          <t>65611</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>49000199</t>
+          <t>15436348</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>SlipperyForester5672</t>
+          <t>Lucas</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
@@ -2792,24 +2792,24 @@
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>1182</t>
+          <t>2484</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>89862</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>38994054</t>
+          <t>54941706</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>chengnan</t>
+          <t>AlexMenjivar20</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
@@ -2819,24 +2819,24 @@
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1550</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>95765</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>55810157</t>
+          <t>57219176</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Beard</t>
+          <t>青莲道人</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
@@ -2846,24 +2846,24 @@
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1499</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>113106</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>57556179</t>
+          <t>49000199</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>特战新生代英雄</t>
+          <t>SlipperyForester5672</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
@@ -2873,7 +2873,7 @@
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1182</t>
         </is>
       </c>
     </row>
@@ -2885,12 +2885,12 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>1222440</t>
+          <t>38994054</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>"Sneaky Ninja Panda"</t>
+          <t>chengnan</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
@@ -2912,12 +2912,12 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>58340439</t>
+          <t>55810157</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>70qilin</t>
+          <t>Beard</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
@@ -2939,12 +2939,12 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>20372140</t>
+          <t>57556179</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>人山即是仙</t>
+          <t>特战新生代英雄</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
@@ -2966,12 +2966,12 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>58615925</t>
+          <t>1222440</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>齐天的大圣</t>
+          <t>"Sneaky Ninja Panda"</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
@@ -2993,12 +2993,12 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>58641574</t>
+          <t>58340439</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>Player-58641574鱼</t>
+          <t>70qilin</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
@@ -3020,12 +3020,12 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>58743790</t>
+          <t>20372140</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>Ma</t>
+          <t>人山即是仙</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
@@ -3042,54 +3042,54 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>52922</t>
+          <t>999999</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>41849539</t>
+          <t>58615925</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>三号馆馆主</t>
+          <t>齐天的大圣</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>2647</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>42326</t>
+          <t>999999</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>56241637</t>
+          <t>58641574</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>Player-14day</t>
+          <t>Player-58641574鱼</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>2981</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -3101,17 +3101,17 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>47622456</t>
+          <t>58743790</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>伊恩</t>
+          <t>Ma</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
@@ -3123,17 +3123,17 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>56017</t>
+          <t>53074</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>55210350</t>
+          <t>41849539</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>一个过客而已</t>
+          <t>三号馆馆主</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
@@ -3143,24 +3143,24 @@
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>2587</t>
+          <t>2647</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>42587</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>49553719</t>
+          <t>56241637</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>"Oreo Captain Sir"</t>
+          <t>Player-14day</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
@@ -3170,24 +3170,24 @@
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2978</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>86022</t>
+          <t>999999</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>59082827</t>
+          <t>47622456</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>Player-59082827</t>
+          <t>伊恩</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
@@ -3197,24 +3197,24 @@
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>1642</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>93418</t>
+          <t>56234</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>59106471</t>
+          <t>55210350</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>anime</t>
+          <t>一个过客而已</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
@@ -3224,24 +3224,24 @@
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>1500</t>
+          <t>2586</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>101518</t>
+          <t>999999</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>41231396</t>
+          <t>49553719</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>ollsthebro</t>
+          <t>"Oreo Captain Sir"</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
@@ -3251,24 +3251,24 @@
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>1399</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>85798</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>58572199</t>
+          <t>59082827</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>你干嘛～哎呦～</t>
+          <t>Player-59082827</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
@@ -3278,24 +3278,24 @@
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1659</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>93622</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>58766144</t>
+          <t>59106471</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>EquablePrecedence38</t>
+          <t>anime</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
@@ -3305,24 +3305,24 @@
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1500</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>101761</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>29355299</t>
+          <t>41231396</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>Player-29355299</t>
+          <t>ollsthebro</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
@@ -3332,7 +3332,7 @@
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1399</t>
         </is>
       </c>
     </row>
@@ -3344,12 +3344,12 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>58910668</t>
+          <t>58572199</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>BrittleAuthor33</t>
+          <t>你干嘛～哎呦～</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
@@ -3371,12 +3371,12 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>55745105</t>
+          <t>58766144</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>eldeniz</t>
+          <t>EquablePrecedence38</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
@@ -3398,12 +3398,12 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>58174442</t>
+          <t>29355299</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>Player-58174442</t>
+          <t>Player-29355299</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
@@ -3425,12 +3425,12 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>58671339</t>
+          <t>58910668</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>"quang pro"</t>
+          <t>BrittleAuthor33</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
@@ -3452,12 +3452,12 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>59081265</t>
+          <t>55745105</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>爬楼梯</t>
+          <t>eldeniz</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
@@ -3479,17 +3479,17 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>10636651</t>
+          <t>58174442</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>"Ismail Aflou"</t>
+          <t>Player-58174442</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>Chinese</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="E116" t="inlineStr">
@@ -3506,17 +3506,17 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>12648101</t>
+          <t>58671339</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>"player 198827"</t>
+          <t>"quang pro"</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>Chinese</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="E117" t="inlineStr">
@@ -3533,17 +3533,17 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>9195340</t>
+          <t>59081265</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>Namllllllik</t>
+          <t>爬楼梯</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>Chinese</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="E118" t="inlineStr">
@@ -3560,12 +3560,12 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>41848598</t>
+          <t>10636651</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>国家一级保护沙雕</t>
+          <t>"Ismail Aflou"</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
@@ -3587,12 +3587,12 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>15755724</t>
+          <t>12648101</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>"Last Good"</t>
+          <t>"player 198827"</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
@@ -3614,12 +3614,12 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>8850180</t>
+          <t>9195340</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>30624300</t>
+          <t>Namllllllik</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
@@ -3641,12 +3641,12 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>28624723</t>
+          <t>41848598</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>"Woody Shade"</t>
+          <t>国家一级保护沙雕</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
@@ -3668,12 +3668,12 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>6010122</t>
+          <t>15755724</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>"Edward Peng"</t>
+          <t>"Last Good"</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
@@ -3695,20 +3695,101 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
+          <t>8850180</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>30624300</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>Chinese</t>
+        </is>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>999999</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>28624723</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>"Woody Shade"</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>Chinese</t>
+        </is>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>999999</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>6010122</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>"Edward Peng"</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>Chinese</t>
+        </is>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>999999</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
           <t>9913517</t>
         </is>
       </c>
-      <c r="C124" t="inlineStr">
+      <c r="C127" t="inlineStr">
         <is>
           <t>"Kenny Chan"</t>
         </is>
       </c>
-      <c r="D124" t="inlineStr">
+      <c r="D127" t="inlineStr">
         <is>
           <t>Chinese</t>
         </is>
       </c>
-      <c r="E124" t="inlineStr">
+      <c r="E127" t="inlineStr">
         <is>
           <t>0</t>
         </is>

</xml_diff>

<commit_message>
Code updated 23-04-08 20:33:47
</commit_message>
<xml_diff>
--- a/Season_Trophies/87.xlsx
+++ b/Season_Trophies/87.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E113"/>
+  <dimension ref="A1:E111"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -396,7 +396,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>61317</t>
+          <t>61099</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -416,14 +416,14 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2728</t>
+          <t>2744</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>24987</t>
+          <t>24888</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -443,24 +443,24 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>4940</t>
+          <t>4977</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>31145</t>
+          <t>25148</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>55634661</t>
+          <t>47928278</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Opalus</t>
+          <t>"落日幻影 哈哈哈"</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -470,24 +470,24 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>4638</t>
+          <t>4962</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>32576</t>
+          <t>30448</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>45967307</t>
+          <t>55634661</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Ricky</t>
+          <t>Opalus</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -497,24 +497,24 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>4577</t>
+          <t>4699</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>45822</t>
+          <t>33245</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>47928278</t>
+          <t>45967307</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>"落日幻影 哈哈哈"</t>
+          <t>Ricky</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -524,14 +524,14 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>3807</t>
+          <t>4577</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>46460</t>
+          <t>43361</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -551,14 +551,14 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>3736</t>
+          <t>4041</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>49754</t>
+          <t>50004</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -585,7 +585,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>58900</t>
+          <t>59165</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -605,14 +605,14 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2814</t>
+          <t>2813</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>67905</t>
+          <t>68127</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -639,7 +639,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>77071</t>
+          <t>77396</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -666,7 +666,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>96209</t>
+          <t>96266</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -686,7 +686,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1796</t>
+          <t>1813</t>
         </is>
       </c>
     </row>
@@ -720,7 +720,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>13884</t>
+          <t>14055</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -740,14 +740,14 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>5641</t>
+          <t>5656</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>9007</t>
+          <t>9359</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -767,24 +767,24 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>6089</t>
+          <t>6081</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>11068</t>
+          <t>10922</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>53060417</t>
+          <t>49710892</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>㊥老纳信耶稣</t>
+          <t>MMMMMMM</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -794,24 +794,24 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>5914</t>
+          <t>5951</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>11117</t>
+          <t>11768</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>49710892</t>
+          <t>53060417</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>MMMMMMM</t>
+          <t>㊥老纳信耶稣</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -821,14 +821,14 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>5910</t>
+          <t>5873</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>11775</t>
+          <t>12002</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -855,7 +855,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>13020</t>
+          <t>13841</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -875,14 +875,14 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>5721</t>
+          <t>5672</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>18098</t>
+          <t>18695</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -902,24 +902,24 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>5339</t>
+          <t>5335</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>18534</t>
+          <t>19310</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>57531381</t>
+          <t>38809086</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>㊥蝦雞霸丸</t>
+          <t>Kouenᶻᵍˣ</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -929,24 +929,24 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>5314</t>
+          <t>5302</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>18761</t>
+          <t>19803</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>38809086</t>
+          <t>4756174</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Kouenᶻᵍˣ</t>
+          <t>純希です</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -956,24 +956,24 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>5302</t>
+          <t>5275</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>19613</t>
+          <t>14995</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>4756174</t>
+          <t>31495601</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>純希です</t>
+          <t>陈晓军</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -983,14 +983,14 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>5253</t>
+          <t>5580</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>16419</t>
+          <t>17489</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1010,14 +1010,14 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>5443</t>
+          <t>5405</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>16703</t>
+          <t>17603</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1037,24 +1037,24 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>5426</t>
+          <t>5399</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>16654</t>
+          <t>22558</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>31495601</t>
+          <t>54085771</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>陈晓军</t>
+          <t>㊥Matthieu</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1064,24 +1064,24 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>5430</t>
+          <t>5109</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>21131</t>
+          <t>23305</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>54085771</t>
+          <t>55769051</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>㊥Matthieu</t>
+          <t>㊥叮叮当.</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1091,24 +1091,24 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>5163</t>
+          <t>5067</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>22859</t>
+          <t>27758</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>55769051</t>
+          <t>46289694</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>㊥叮叮当.</t>
+          <t>㊥Vincent</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1118,24 +1118,24 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>5058</t>
+          <t>4827</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>27920</t>
+          <t>29302</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>46289694</t>
+          <t>55860890</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>㊥Vincent</t>
+          <t>㊥Ethan</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1145,24 +1145,24 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>4790</t>
+          <t>4751</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>28531</t>
+          <t>31873</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>55860890</t>
+          <t>3649043</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>㊥Ethan</t>
+          <t>Dj6106</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1172,24 +1172,24 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>4759</t>
+          <t>4637</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>30911</t>
+          <t>34275</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>3649043</t>
+          <t>56585361</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Dj6106</t>
+          <t>"㊥ go策划我要ali"</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1199,24 +1199,24 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>4648</t>
+          <t>4526</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>34480</t>
+          <t>35576</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>56732705</t>
+          <t>58839983</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>时间温柔皆遗憾</t>
+          <t>每逢佳节胖六斤</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1226,24 +1226,24 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>4487</t>
+          <t>4463</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>35227</t>
+          <t>35536</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>58839983</t>
+          <t>56732705</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>每逢佳节胖六斤</t>
+          <t>时间温柔皆遗憾</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1253,24 +1253,24 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>4449</t>
+          <t>4465</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>35971</t>
+          <t>40565</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>56585361</t>
+          <t>58408326</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>"㊥ go策划我要ali"</t>
+          <t>"Killer Bee"</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1280,24 +1280,24 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>4411</t>
+          <t>4200</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>40284</t>
+          <t>43096</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>58408326</t>
+          <t>1304123</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>"Killer Bee"</t>
+          <t>Cccccccccccc</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1307,24 +1307,24 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>4192</t>
+          <t>4059</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>42490</t>
+          <t>6907</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>1304123</t>
+          <t>4493731</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Cccccccccccc</t>
+          <t>Player-1527362</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1334,24 +1334,24 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>4075</t>
+          <t>6326</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>6678</t>
+          <t>7889</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>4493731</t>
+          <t>7852598</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Player-1527362</t>
+          <t>seiji</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1361,24 +1361,24 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>6332</t>
+          <t>6217</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>7675</t>
+          <t>10705</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>7852598</t>
+          <t>11582001</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>seiji</t>
+          <t>iMinatoX4</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1388,24 +1388,24 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>6217</t>
+          <t>5971</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>9442</t>
+          <t>14896</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>4229136</t>
+          <t>56133764</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>"totoro wu"</t>
+          <t>ustcarter</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1415,24 +1415,24 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>6052</t>
+          <t>5588</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>10410</t>
+          <t>15876</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>11582001</t>
+          <t>55317038</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>iMinatoX4</t>
+          <t>necman12345</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1442,24 +1442,24 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>5971</t>
+          <t>5513</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>13391</t>
+          <t>16730</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>56133764</t>
+          <t>6809364</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>ustcarter</t>
+          <t>"Scorp IP"</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1469,24 +1469,24 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>5684</t>
+          <t>5454</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>16481</t>
+          <t>21297</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>6809364</t>
+          <t>38995116</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>"Scorp IP"</t>
+          <t>"Ramesh Pavai Nam"</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -1496,24 +1496,24 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>5439</t>
+          <t>5191</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>18250</t>
+          <t>22647</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>55317038</t>
+          <t>54778421</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>necman12345</t>
+          <t>Emma</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -1523,24 +1523,24 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>5330</t>
+          <t>5103</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>21236</t>
+          <t>25782</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>38995116</t>
+          <t>31401481</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>"Ramesh Pavai Nam"</t>
+          <t>Player-31401481</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -1550,24 +1550,24 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>5156</t>
+          <t>4928</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>22024</t>
+          <t>31535</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>54778421</t>
+          <t>47459684</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Emma</t>
+          <t>㊥阿闹切克闹</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -1577,24 +1577,24 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>5110</t>
+          <t>4652</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>24724</t>
+          <t>32608</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>31401481</t>
+          <t>56573048</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Player-31401481</t>
+          <t>Xiaotian</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1604,24 +1604,24 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>4953</t>
+          <t>4605</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>31107</t>
+          <t>33253</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>47459684</t>
+          <t>32316256</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>㊥阿闹切克闹</t>
+          <t>"秋の風 .."</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -1631,24 +1631,24 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>4640</t>
+          <t>4577</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>33110</t>
+          <t>34713</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>32316256</t>
+          <t>56379103</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>"秋の風 .."</t>
+          <t>Globalking1001</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -1658,24 +1658,24 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>4553</t>
+          <t>4506</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>33505</t>
+          <t>39127</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>56573048</t>
+          <t>38893233</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Xiaotian</t>
+          <t>"快乐 二哈"</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -1685,24 +1685,24 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>4533</t>
+          <t>4273</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>33677</t>
+          <t>39815</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>56379103</t>
+          <t>24733875</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Globalking1001</t>
+          <t>龍少</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -1712,24 +1712,24 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>4525</t>
+          <t>4237</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>39237</t>
+          <t>40898</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>38893233</t>
+          <t>58203298</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>"快乐 二哈"</t>
+          <t>权旨qua</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -1739,24 +1739,24 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>4244</t>
+          <t>4183</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>39365</t>
+          <t>41602</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>24733875</t>
+          <t>56500325</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>龍少</t>
+          <t>haruharuyukizg9735</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -1766,24 +1766,24 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>4237</t>
+          <t>4145</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>40639</t>
+          <t>42516</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>58203298</t>
+          <t>57813281</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>权旨qua</t>
+          <t>XAUEN</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -1793,24 +1793,24 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>4175</t>
+          <t>4094</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>40983</t>
+          <t>44402</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>56500325</t>
+          <t>50837459</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>haruharuyukizg9735</t>
+          <t>NINE日</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -1820,24 +1820,24 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>4157</t>
+          <t>3990</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>41898</t>
+          <t>45693</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>57813281</t>
+          <t>52997727</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>XAUEN</t>
+          <t>larios</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -1847,24 +1847,24 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>4107</t>
+          <t>3861</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>44059</t>
+          <t>48613</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>50837459</t>
+          <t>48634530</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>NINE日</t>
+          <t>leezhenrui</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -1874,24 +1874,24 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>3991</t>
+          <t>3519</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>45550</t>
+          <t>62779</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>52997727</t>
+          <t>1550355</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>larios</t>
+          <t>"皓茵 世界"</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -1901,78 +1901,78 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>3839</t>
+          <t>2691</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>48657</t>
+          <t>17872</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>48634530</t>
+          <t>31134300</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>leezhenrui</t>
+          <t>McMaX</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>3491</t>
+          <t>5385</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>62522</t>
+          <t>60681</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>1550355</t>
+          <t>43281368</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>"皓茵 世界"</t>
+          <t>xhs2763</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>2691</t>
+          <t>2758</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>17267</t>
+          <t>69214</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>31134300</t>
+          <t>44378757</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>McMaX</t>
+          <t>"NᵉᵗʰᵉʳDʳⁱᶠᵗᵉʳ ㊥"</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -1982,24 +1982,24 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>5392</t>
+          <t>2539</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>60859</t>
+          <t>999999</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>43281368</t>
+          <t>48738257</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>xhs2763</t>
+          <t>死亡洲际跳蛋</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -2009,24 +2009,24 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>2743</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>68979</t>
+          <t>24050</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>44378757</t>
+          <t>25479797</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>"NᵉᵗʰᵉʳDʳⁱᶠᵗᵉʳ ㊥"</t>
+          <t>"Mohamed Alnaqbi"</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -2036,24 +2036,24 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>2539</t>
+          <t>5026</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>27090</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>48738257</t>
+          <t>44708798</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>死亡洲际跳蛋</t>
+          <t>"㊥ mythgod"</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -2063,24 +2063,24 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>4858</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>23407</t>
+          <t>49549</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>25479797</t>
+          <t>54588689</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>"Mohamed Alnaqbi"</t>
+          <t>㊥墨衍枫迹☜</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -2090,24 +2090,24 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>5026</t>
+          <t>3425</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>26501</t>
+          <t>56739</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>44708798</t>
+          <t>28855852</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>"㊥ mythgod"</t>
+          <t>tiger</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -2117,24 +2117,24 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>4859</t>
+          <t>2916</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>49671</t>
+          <t>21125</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>54588689</t>
+          <t>18082891</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>㊥墨衍枫迹☜</t>
+          <t>Michael</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -2144,24 +2144,24 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>3389</t>
+          <t>5202</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>56492</t>
+          <t>31087</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>28855852</t>
+          <t>55499394</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>tiger</t>
+          <t>Player-55499394</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -2171,24 +2171,24 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>2916</t>
+          <t>4672</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>22401</t>
+          <t>50249</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>18082891</t>
+          <t>47430231</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Michael</t>
+          <t>Kentantrino</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -2198,24 +2198,24 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>5086</t>
+          <t>3358</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>34201</t>
+          <t>52558</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>55499394</t>
+          <t>11645391</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Player-55499394</t>
+          <t>"omar omar"</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -2225,24 +2225,24 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>4501</t>
+          <t>3168</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>49974</t>
+          <t>52704</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>47430231</t>
+          <t>56700848</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Kentantrino</t>
+          <t>工口漫画老师</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -2252,24 +2252,24 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>3362</t>
+          <t>3158</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>52296</t>
+          <t>56126</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>11645391</t>
+          <t>3391765</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>"omar omar"</t>
+          <t>马er</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -2279,24 +2279,24 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>3169</t>
+          <t>2945</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>52444</t>
+          <t>61240</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>56700848</t>
+          <t>9718882</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>工口漫画老师</t>
+          <t>小霸王2021</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -2306,24 +2306,24 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>3158</t>
+          <t>2739</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>55860</t>
+          <t>74795</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>3391765</t>
+          <t>15436348</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>马er</t>
+          <t>Lucas</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -2333,24 +2333,24 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>2946</t>
+          <t>2439</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>60967</t>
+          <t>104459</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>9718882</t>
+          <t>54941706</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>小霸王2021</t>
+          <t>AlexMenjivar20</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -2360,24 +2360,24 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>2739</t>
+          <t>1612</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>74542</t>
+          <t>118930</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>15436348</t>
+          <t>57219176</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Lucas</t>
+          <t>青莲道人</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -2387,24 +2387,24 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>2439</t>
+          <t>1457</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>103860</t>
+          <t>140576</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>54941706</t>
+          <t>49000199</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>AlexMenjivar20</t>
+          <t>SlipperyForester5672</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -2414,24 +2414,24 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>1612</t>
+          <t>1225</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>118260</t>
+          <t>999999</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>57219176</t>
+          <t>38994054</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>青莲道人</t>
+          <t>chengnan</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -2441,24 +2441,24 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>1457</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>139341</t>
+          <t>999999</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>49000199</t>
+          <t>55810157</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>SlipperyForester5672</t>
+          <t>Beard</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -2468,7 +2468,7 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>1227</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2480,12 +2480,12 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>38994054</t>
+          <t>57556179</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>chengnan</t>
+          <t>特战新生代英雄</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -2507,12 +2507,12 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>55810157</t>
+          <t>1222440</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Beard</t>
+          <t>"Sneaky Ninja Panda"</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -2534,12 +2534,12 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>57556179</t>
+          <t>58340439</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>特战新生代英雄</t>
+          <t>70qilin</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -2561,12 +2561,12 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>1222440</t>
+          <t>20372140</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>"Sneaky Ninja Panda"</t>
+          <t>人山即是仙</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -2588,12 +2588,12 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>58340439</t>
+          <t>58615925</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>70qilin</t>
+          <t>齐天的大圣</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
@@ -2615,12 +2615,12 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>20372140</t>
+          <t>58641574</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>人山即是仙</t>
+          <t>Player-58641574鱼</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -2642,12 +2642,12 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>58615925</t>
+          <t>58743790</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>齐天的大圣</t>
+          <t>Ma</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
@@ -2664,71 +2664,71 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>53543</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>58641574</t>
+          <t>41849539</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Player-58641574鱼</t>
+          <t>三号馆馆主</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>3095</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>44489</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>58743790</t>
+          <t>56241637</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Ma</t>
+          <t>Player-14day</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>3986</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>53242</t>
+          <t>999999</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>41849539</t>
+          <t>47622456</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>三号馆馆主</t>
+          <t>伊恩</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
@@ -2738,24 +2738,24 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>3099</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>44115</t>
+          <t>57134</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>56241637</t>
+          <t>55210350</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Player-14day</t>
+          <t>一个过客而已</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
@@ -2765,7 +2765,7 @@
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>3989</t>
+          <t>2899</t>
         </is>
       </c>
     </row>
@@ -2777,12 +2777,12 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>47622456</t>
+          <t>49553719</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>伊恩</t>
+          <t>"Oreo Captain Sir"</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
@@ -2799,17 +2799,17 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>57035</t>
+          <t>89000</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>55210350</t>
+          <t>58671339</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>一个过客而已</t>
+          <t>"quang pro"</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
@@ -2819,24 +2819,24 @@
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>2892</t>
+          <t>2057</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>89647</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>49553719</t>
+          <t>59082827</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>"Oreo Captain Sir"</t>
+          <t>Player-59082827</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
@@ -2846,24 +2846,24 @@
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2043</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>88521</t>
+          <t>104186</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>58671339</t>
+          <t>59106471</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>"quang pro"</t>
+          <t>anime</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
@@ -2873,24 +2873,24 @@
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>2059</t>
+          <t>1616</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>88871</t>
+          <t>123997</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>59082827</t>
+          <t>41231396</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>Player-59082827</t>
+          <t>ollsthebro</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
@@ -2900,24 +2900,24 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>2052</t>
+          <t>1397</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>103584</t>
+          <t>140117</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>59106471</t>
+          <t>59112086</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>anime</t>
+          <t>sigma</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
@@ -2927,24 +2927,24 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>1616</t>
+          <t>1229</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>123256</t>
+          <t>211276</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>41231396</t>
+          <t>55745105</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>ollsthebro</t>
+          <t>eldeniz</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
@@ -2954,24 +2954,24 @@
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>1397</t>
+          <t>1000</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>139096</t>
+          <t>999999</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>59112086</t>
+          <t>58572199</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>sigma</t>
+          <t>你干嘛～哎呦～</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
@@ -2981,24 +2981,24 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>1229</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>208684</t>
+          <t>999999</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>55745105</t>
+          <t>58766144</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>eldeniz</t>
+          <t>EquablePrecedence38</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
@@ -3008,7 +3008,7 @@
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>1000</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -3020,12 +3020,12 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>58572199</t>
+          <t>29355299</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>你干嘛～哎呦～</t>
+          <t>Player-29355299</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
@@ -3047,12 +3047,12 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>58766144</t>
+          <t>58910668</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>EquablePrecedence38</t>
+          <t>BrittleAuthor33</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
@@ -3074,12 +3074,12 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>29355299</t>
+          <t>58174442</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>Player-29355299</t>
+          <t>Player-58174442</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
@@ -3101,12 +3101,12 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>58910668</t>
+          <t>59081265</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>BrittleAuthor33</t>
+          <t>爬楼梯</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
@@ -3123,27 +3123,27 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>52583</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>58174442</t>
+          <t>41848598</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>Player-58174442</t>
+          <t>国家一级保护沙雕</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>Chinese</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>3166</t>
         </is>
       </c>
     </row>
@@ -3155,17 +3155,17 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>59081265</t>
+          <t>12648101</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>爬楼梯</t>
+          <t>"player 198827"</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>Chinese</t>
         </is>
       </c>
       <c r="E104" t="inlineStr">
@@ -3177,17 +3177,17 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>52330</t>
+          <t>999999</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>41848598</t>
+          <t>9195340</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>国家一级保护沙雕</t>
+          <t>Namllllllik</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
@@ -3197,7 +3197,7 @@
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>3166</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -3209,12 +3209,12 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>12648101</t>
+          <t>15755724</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>"player 198827"</t>
+          <t>"Last Good"</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
@@ -3236,12 +3236,12 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>9195340</t>
+          <t>8850180</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>Namllllllik</t>
+          <t>30624300</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
@@ -3263,12 +3263,12 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>15755724</t>
+          <t>28624723</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>"Last Good"</t>
+          <t>"Woody Shade"</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
@@ -3290,12 +3290,12 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>8850180</t>
+          <t>6010122</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>30624300</t>
+          <t>"Edward Peng"</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
@@ -3317,12 +3317,12 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>28624723</t>
+          <t>9913517</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>"Woody Shade"</t>
+          <t>"Kenny Chan"</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
@@ -3344,12 +3344,12 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>6010122</t>
+          <t>10636651</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>"Edward Peng"</t>
+          <t>"Ismail Aflou"</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
@@ -3358,60 +3358,6 @@
         </is>
       </c>
       <c r="E111" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" t="inlineStr">
-        <is>
-          <t>999999</t>
-        </is>
-      </c>
-      <c r="B112" t="inlineStr">
-        <is>
-          <t>9913517</t>
-        </is>
-      </c>
-      <c r="C112" t="inlineStr">
-        <is>
-          <t>"Kenny Chan"</t>
-        </is>
-      </c>
-      <c r="D112" t="inlineStr">
-        <is>
-          <t>Chinese</t>
-        </is>
-      </c>
-      <c r="E112" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" t="inlineStr">
-        <is>
-          <t>999999</t>
-        </is>
-      </c>
-      <c r="B113" t="inlineStr">
-        <is>
-          <t>10636651</t>
-        </is>
-      </c>
-      <c r="C113" t="inlineStr">
-        <is>
-          <t>"Ismail Aflou"</t>
-        </is>
-      </c>
-      <c r="D113" t="inlineStr">
-        <is>
-          <t>Chinese</t>
-        </is>
-      </c>
-      <c r="E113" t="inlineStr">
         <is>
           <t>0</t>
         </is>

</xml_diff>

<commit_message>
Code updated 23-04-09 11:31:03
</commit_message>
<xml_diff>
--- a/Season_Trophies/87.xlsx
+++ b/Season_Trophies/87.xlsx
@@ -396,17 +396,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>61099</t>
+          <t>68448</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>42542275</t>
+          <t>6510348</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>"同 风 雨"</t>
+          <t>Bonpoisson</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -416,24 +416,24 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2744</t>
+          <t>2559</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>24888</t>
+          <t>50419</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>37069173</t>
+          <t>7587898</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>詹toniii</t>
+          <t>藍精靈ᶻᵍˣ</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -443,24 +443,24 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>4977</t>
+          <t>3380</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>25148</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>47928278</t>
+          <t>23687250</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>"落日幻影 哈哈哈"</t>
+          <t>"jetlijp ᶻᵍˣ"</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -470,24 +470,24 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>4962</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>30448</t>
+          <t>26330</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>55634661</t>
+          <t>37069173</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Opalus</t>
+          <t>詹toniii</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -497,24 +497,24 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>4699</t>
+          <t>4956</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>33245</t>
+          <t>61500</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>45967307</t>
+          <t>42542275</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Ricky</t>
+          <t>"同 风 雨"</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -524,24 +524,24 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>4577</t>
+          <t>2742</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>43361</t>
+          <t>34178</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>20737010</t>
+          <t>45967307</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>混着玩...</t>
+          <t>Ricky</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -551,24 +551,24 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>4041</t>
+          <t>4577</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>50004</t>
+          <t>26011</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>7587898</t>
+          <t>47928278</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>藍精靈ᶻᵍˣ</t>
+          <t>"落日幻影 哈哈哈"</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -578,24 +578,24 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>3380</t>
+          <t>4975</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>59165</t>
+          <t>29878</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>59095922</t>
+          <t>55634661</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>xxxx7</t>
+          <t>Opalus</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -605,24 +605,24 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2813</t>
+          <t>4769</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>68127</t>
+          <t>77896</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>6510348</t>
+          <t>59093405</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Bonpoisson</t>
+          <t>永恒不朽6</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -632,24 +632,24 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2559</t>
+          <t>2330</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>77396</t>
+          <t>59515</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>59093405</t>
+          <t>59095922</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>永恒不朽6</t>
+          <t>xxxx7</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -659,14 +659,14 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2330</t>
+          <t>2813</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>96266</t>
+          <t>96591</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -686,51 +686,51 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1813</t>
+          <t>1824</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>41213</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>23687250</t>
+          <t>1304123</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>"jetlijp ᶻᵍˣ"</t>
+          <t>Cccccccccccc</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>4198</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>14055</t>
+          <t>63134</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>37861953</t>
+          <t>1550355</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>"Durex ๑• . •๑"</t>
+          <t>"皓茵 世界"</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -740,24 +740,24 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>5656</t>
+          <t>2691</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>9359</t>
+          <t>33112</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>47131129</t>
+          <t>3649043</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>NAM</t>
+          <t>Dj6106</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -767,24 +767,24 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>6081</t>
+          <t>4621</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>10922</t>
+          <t>6559</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>49710892</t>
+          <t>4493731</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>MMMMMMM</t>
+          <t>Player-1527362</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -794,24 +794,24 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>5951</t>
+          <t>6537</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>11768</t>
+          <t>18917</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>53060417</t>
+          <t>4756174</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>㊥老纳信耶稣</t>
+          <t>純希です</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -821,24 +821,24 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>5873</t>
+          <t>5402</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>12002</t>
+          <t>15872</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>47146736</t>
+          <t>6809364</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>"HK 品瑜"</t>
+          <t>"Scorp IP"</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -848,24 +848,24 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>5848</t>
+          <t>5602</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>13841</t>
+          <t>6803</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>53520939</t>
+          <t>7852598</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>㊥虎哥tiger</t>
+          <t>seiji</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -875,24 +875,24 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>5672</t>
+          <t>6503</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>18695</t>
+          <t>15117</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>12333251</t>
+          <t>8057001</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>"㊌ Mingxuan"</t>
+          <t>㊥兵者诡道也</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -902,24 +902,24 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>5335</t>
+          <t>5665</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>19310</t>
+          <t>9844</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>38809086</t>
+          <t>11582001</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Kouenᶻᵍˣ</t>
+          <t>iMinatoX4</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -929,24 +929,24 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>5302</t>
+          <t>6176</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>19803</t>
+          <t>17405</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>4756174</t>
+          <t>12333251</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>純希です</t>
+          <t>"㊌ Mingxuan"</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -956,24 +956,24 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>5275</t>
+          <t>5494</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>14995</t>
+          <t>43822</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>31495601</t>
+          <t>20737010</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>陈晓军</t>
+          <t>混着玩...</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -983,24 +983,24 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>5580</t>
+          <t>4041</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>17489</t>
+          <t>40471</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>8057001</t>
+          <t>24733875</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>㊥兵者诡道也</t>
+          <t>龍少</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1010,24 +1010,24 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>5405</t>
+          <t>4237</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>17603</t>
+          <t>24860</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>54698813</t>
+          <t>31401481</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>閃亮唐老鴨</t>
+          <t>Player-31401481</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1037,24 +1037,24 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>5399</t>
+          <t>5041</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>22558</t>
+          <t>16179</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>54085771</t>
+          <t>31495601</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>㊥Matthieu</t>
+          <t>陈晓军</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1064,24 +1064,24 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>5109</t>
+          <t>5579</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>23305</t>
+          <t>26710</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>55769051</t>
+          <t>32316256</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>㊥叮叮当.</t>
+          <t>"秋の風 .."</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1091,24 +1091,24 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>5067</t>
+          <t>4934</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>27758</t>
+          <t>14358</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>46289694</t>
+          <t>37861953</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>㊥Vincent</t>
+          <t>"Durex ๑• . •๑"</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1118,24 +1118,24 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>4827</t>
+          <t>5732</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>29302</t>
+          <t>19623</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>55860890</t>
+          <t>38809086</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>㊥Ethan</t>
+          <t>Kouenᶻᵍˣ</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1145,24 +1145,24 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>4751</t>
+          <t>5363</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>31873</t>
+          <t>33379</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>3649043</t>
+          <t>38893233</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Dj6106</t>
+          <t>"快乐 二哈"</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1172,24 +1172,24 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>4637</t>
+          <t>4610</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>34275</t>
+          <t>22824</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>56585361</t>
+          <t>38995116</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>"㊥ go策划我要ali"</t>
+          <t>"Ramesh Pavai Nam"</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1199,24 +1199,24 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>4526</t>
+          <t>5176</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>35576</t>
+          <t>29237</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>58839983</t>
+          <t>46289694</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>每逢佳节胖六斤</t>
+          <t>㊥Vincent</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1226,24 +1226,24 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>4463</t>
+          <t>4803</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>35536</t>
+          <t>8450</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>56732705</t>
+          <t>47131129</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>时间温柔皆遗憾</t>
+          <t>NAM</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1253,24 +1253,24 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>4465</t>
+          <t>6303</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>40565</t>
+          <t>10954</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>58408326</t>
+          <t>47146736</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>"Killer Bee"</t>
+          <t>"HK 品瑜"</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1280,24 +1280,24 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>4200</t>
+          <t>6095</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>43096</t>
+          <t>31611</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>1304123</t>
+          <t>47459684</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Cccccccccccc</t>
+          <t>㊥阿闹切克闹</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1307,24 +1307,24 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>4059</t>
+          <t>4689</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>6907</t>
+          <t>48871</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>4493731</t>
+          <t>48634530</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Player-1527362</t>
+          <t>leezhenrui</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1334,24 +1334,24 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>6326</t>
+          <t>3532</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>7889</t>
+          <t>12399</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>7852598</t>
+          <t>49710892</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>seiji</t>
+          <t>MMMMMMM</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1361,24 +1361,24 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>6217</t>
+          <t>5973</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>10705</t>
+          <t>40334</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>11582001</t>
+          <t>50837459</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>iMinatoX4</t>
+          <t>NINE日</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1388,24 +1388,24 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>5971</t>
+          <t>4244</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>14896</t>
+          <t>46108</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>56133764</t>
+          <t>52997727</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>ustcarter</t>
+          <t>larios</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1415,24 +1415,24 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>5588</t>
+          <t>3861</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>15876</t>
+          <t>11450</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>55317038</t>
+          <t>53060417</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>necman12345</t>
+          <t>㊥老纳信耶稣</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1442,24 +1442,24 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>5513</t>
+          <t>6057</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>16730</t>
+          <t>13080</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>6809364</t>
+          <t>53520939</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>"Scorp IP"</t>
+          <t>㊥虎哥tiger</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1469,24 +1469,24 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>5454</t>
+          <t>5869</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>21297</t>
+          <t>21387</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>38995116</t>
+          <t>54085771</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>"Ramesh Pavai Nam"</t>
+          <t>㊥Matthieu</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -1496,24 +1496,24 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>5191</t>
+          <t>5264</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>22647</t>
+          <t>16822</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>54778421</t>
+          <t>54698813</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Emma</t>
+          <t>閃亮唐老鴨</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -1523,24 +1523,24 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>5103</t>
+          <t>5532</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>25782</t>
+          <t>23945</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>31401481</t>
+          <t>54778421</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Player-31401481</t>
+          <t>Emma</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -1550,24 +1550,24 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>4928</t>
+          <t>5095</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>31535</t>
+          <t>18273</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>47459684</t>
+          <t>55317038</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>㊥阿闹切克闹</t>
+          <t>necman12345</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -1577,24 +1577,24 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>4652</t>
+          <t>5438</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>32608</t>
+          <t>22210</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>56573048</t>
+          <t>55769051</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Xiaotian</t>
+          <t>㊥叮叮当.</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1604,24 +1604,24 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>4605</t>
+          <t>5220</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>33253</t>
+          <t>26678</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>32316256</t>
+          <t>55860890</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>"秋の風 .."</t>
+          <t>㊥Ethan</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -1631,24 +1631,24 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>4577</t>
+          <t>4936</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>34713</t>
+          <t>13377</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>56379103</t>
+          <t>56133764</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Globalking1001</t>
+          <t>ustcarter</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -1658,24 +1658,24 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>4506</t>
+          <t>5828</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>39127</t>
+          <t>34637</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>38893233</t>
+          <t>56379103</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>"快乐 二哈"</t>
+          <t>Globalking1001</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -1685,24 +1685,24 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>4273</t>
+          <t>4556</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>39815</t>
+          <t>42226</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>24733875</t>
+          <t>56500325</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>龍少</t>
+          <t>haruharuyukizg9735</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -1712,24 +1712,24 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>4237</t>
+          <t>4139</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>40898</t>
+          <t>33228</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>58203298</t>
+          <t>56573048</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>权旨qua</t>
+          <t>Xiaotian</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -1739,24 +1739,24 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>4183</t>
+          <t>4616</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>41602</t>
+          <t>35765</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>56500325</t>
+          <t>56585361</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>haruharuyukizg9735</t>
+          <t>"㊥ go策划我要ali"</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -1766,24 +1766,24 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>4145</t>
+          <t>4500</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>42516</t>
+          <t>33752</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>57813281</t>
+          <t>56732705</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>XAUEN</t>
+          <t>时间温柔皆遗憾</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -1793,24 +1793,24 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>4094</t>
+          <t>4596</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>44402</t>
+          <t>43601</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>50837459</t>
+          <t>57813281</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>NINE日</t>
+          <t>XAUEN</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -1820,24 +1820,24 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>3990</t>
+          <t>4055</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>45693</t>
+          <t>40812</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>52997727</t>
+          <t>58203298</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>larios</t>
+          <t>权旨qua</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -1847,24 +1847,24 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>3861</t>
+          <t>4218</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>48613</t>
+          <t>42512</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>48634530</t>
+          <t>58408326</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>leezhenrui</t>
+          <t>"Killer Bee"</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -1874,24 +1874,24 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>3519</t>
+          <t>4123</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>62779</t>
+          <t>35662</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>1550355</t>
+          <t>58839983</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>"皓茵 世界"</t>
+          <t>每逢佳节胖六斤</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -1901,24 +1901,24 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>2691</t>
+          <t>4506</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>17872</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>31134300</t>
+          <t>1222440</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>McMaX</t>
+          <t>"Sneaky Ninja Panda"</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -1928,24 +1928,24 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>5385</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>60681</t>
+          <t>56548</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>43281368</t>
+          <t>3391765</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>xhs2763</t>
+          <t>马er</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -1955,24 +1955,24 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>2758</t>
+          <t>2944</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>69214</t>
+          <t>61634</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>44378757</t>
+          <t>9718882</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>"NᵉᵗʰᵉʳDʳⁱᶠᵗᵉʳ ㊥"</t>
+          <t>小霸王2021</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -1982,24 +1982,24 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>2539</t>
+          <t>2737</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>53010</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>48738257</t>
+          <t>11645391</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>死亡洲际跳蛋</t>
+          <t>"omar omar"</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -2009,24 +2009,24 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>3168</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>24050</t>
+          <t>75222</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>25479797</t>
+          <t>15436348</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>"Mohamed Alnaqbi"</t>
+          <t>Lucas</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -2036,24 +2036,24 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>5026</t>
+          <t>2439</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>27090</t>
+          <t>21815</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>44708798</t>
+          <t>18082891</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>"㊥ mythgod"</t>
+          <t>Michael</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -2063,24 +2063,24 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>4858</t>
+          <t>5241</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>49549</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>54588689</t>
+          <t>20372140</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>㊥墨衍枫迹☜</t>
+          <t>人山即是仙</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -2090,24 +2090,24 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>3425</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>56739</t>
+          <t>22548</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>28855852</t>
+          <t>25479797</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>tiger</t>
+          <t>"Mohamed Alnaqbi"</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -2117,24 +2117,24 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>2916</t>
+          <t>5200</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>21125</t>
+          <t>57168</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>18082891</t>
+          <t>28855852</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Michael</t>
+          <t>tiger</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -2144,24 +2144,24 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>5202</t>
+          <t>2916</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>31087</t>
+          <t>17211</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>55499394</t>
+          <t>31134300</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Player-55499394</t>
+          <t>McMaX</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -2171,24 +2171,24 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>4672</t>
+          <t>5509</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>50249</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>47430231</t>
+          <t>38994054</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Kentantrino</t>
+          <t>chengnan</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -2198,24 +2198,24 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>3358</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>52558</t>
+          <t>61067</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>11645391</t>
+          <t>43281368</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>"omar omar"</t>
+          <t>xhs2763</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -2225,24 +2225,24 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>3168</t>
+          <t>2757</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>52704</t>
+          <t>69540</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>56700848</t>
+          <t>44378757</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>工口漫画老师</t>
+          <t>"NᵉᵗʰᵉʳDʳⁱᶠᵗᵉʳ ㊥"</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -2252,24 +2252,24 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>3158</t>
+          <t>2539</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>56126</t>
+          <t>27472</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>3391765</t>
+          <t>44708798</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>马er</t>
+          <t>"㊥ mythgod"</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -2279,24 +2279,24 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>2945</t>
+          <t>4891</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>61240</t>
+          <t>50718</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>9718882</t>
+          <t>47430231</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>小霸王2021</t>
+          <t>Kentantrino</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -2306,24 +2306,24 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>2739</t>
+          <t>3355</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>74795</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>15436348</t>
+          <t>48738257</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Lucas</t>
+          <t>死亡洲际跳蛋</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -2333,24 +2333,24 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>2439</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>104459</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>54941706</t>
+          <t>49000199</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>AlexMenjivar20</t>
+          <t>SlipperyForester5672</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -2360,24 +2360,24 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>1612</t>
+          <t>1225</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>118930</t>
+          <t>49816</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>57219176</t>
+          <t>54588689</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>青莲道人</t>
+          <t>㊥墨衍枫迹☜</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -2387,24 +2387,24 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>1457</t>
+          <t>3440</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>140576</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>49000199</t>
+          <t>54941706</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>SlipperyForester5672</t>
+          <t>AlexMenjivar20</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -2414,24 +2414,24 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>1225</t>
+          <t>1612</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>32423</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>38994054</t>
+          <t>55499394</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>chengnan</t>
+          <t>Player-55499394</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -2441,14 +2441,14 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>4653</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2475,17 +2475,17 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>52751</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>57556179</t>
+          <t>56700848</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>特战新生代英雄</t>
+          <t>工口漫画老师</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -2495,24 +2495,24 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>3187</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>1222440</t>
+          <t>57219176</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>"Sneaky Ninja Panda"</t>
+          <t>青莲道人</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -2522,24 +2522,24 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1455</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>58340439</t>
+          <t>57556179</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>70qilin</t>
+          <t>特战新生代英雄</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -2556,17 +2556,17 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>20372140</t>
+          <t>58340439</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>人山即是仙</t>
+          <t>70qilin</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -2583,7 +2583,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -2610,7 +2610,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -2637,7 +2637,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2664,17 +2664,17 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>53543</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>41849539</t>
+          <t>29355299</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>三号馆馆主</t>
+          <t>Player-29355299</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
@@ -2684,24 +2684,24 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>3095</t>
+          <t>999</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>44489</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>56241637</t>
+          <t>41231396</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Player-14day</t>
+          <t>ollsthebro</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
@@ -2711,24 +2711,24 @@
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>3986</t>
+          <t>1397</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>53619</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>47622456</t>
+          <t>41849539</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>伊恩</t>
+          <t>三号馆馆主</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
@@ -2738,24 +2738,24 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>3122</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>57134</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>55210350</t>
+          <t>47622456</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>一个过客而已</t>
+          <t>伊恩</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
@@ -2765,14 +2765,14 @@
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>2899</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -2799,17 +2799,17 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>89000</t>
+          <t>57531</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>58671339</t>
+          <t>55210350</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>"quang pro"</t>
+          <t>一个过客而已</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
@@ -2819,24 +2819,24 @@
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>2057</t>
+          <t>2899</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>89647</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>59082827</t>
+          <t>55745105</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Player-59082827</t>
+          <t>eldeniz</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
@@ -2846,24 +2846,24 @@
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>2043</t>
+          <t>1000</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>104186</t>
+          <t>45019</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>59106471</t>
+          <t>56241637</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>anime</t>
+          <t>Player-14day</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
@@ -2873,24 +2873,24 @@
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>1616</t>
+          <t>3982</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>123997</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>41231396</t>
+          <t>58174442</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>ollsthebro</t>
+          <t>Player-58174442</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
@@ -2900,24 +2900,24 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>1397</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>140117</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>59112086</t>
+          <t>58572199</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>sigma</t>
+          <t>你干嘛～哎呦～</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
@@ -2927,24 +2927,24 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>1229</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>211276</t>
+          <t>89567</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>55745105</t>
+          <t>58671339</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>eldeniz</t>
+          <t>"quang pro"</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
@@ -2954,24 +2954,24 @@
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>1000</t>
+          <t>2057</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>58572199</t>
+          <t>58766144</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>你干嘛～哎呦～</t>
+          <t>EquablePrecedence38</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
@@ -2988,17 +2988,17 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>58766144</t>
+          <t>58910668</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>EquablePrecedence38</t>
+          <t>BrittleAuthor33</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
@@ -3015,17 +3015,17 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>29355299</t>
+          <t>59081265</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>Player-29355299</t>
+          <t>爬楼梯</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
@@ -3042,17 +3042,17 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>89455</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>58910668</t>
+          <t>59082827</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>BrittleAuthor33</t>
+          <t>Player-59082827</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
@@ -3062,24 +3062,24 @@
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2059</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>58174442</t>
+          <t>59106471</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>Player-58174442</t>
+          <t>anime</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
@@ -3089,24 +3089,24 @@
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1616</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>59081265</t>
+          <t>59112086</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>爬楼梯</t>
+          <t>sigma</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
@@ -3116,24 +3116,24 @@
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1229</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>52583</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>41848598</t>
+          <t>6010122</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>国家一级保护沙雕</t>
+          <t>"Edward Peng"</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
@@ -3143,24 +3143,24 @@
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>3166</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>12648101</t>
+          <t>8850180</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>"player 198827"</t>
+          <t>30624300</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
@@ -3177,7 +3177,7 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
@@ -3204,17 +3204,17 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>15755724</t>
+          <t>9913517</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>"Last Good"</t>
+          <t>"Kenny Chan"</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
@@ -3231,17 +3231,17 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>8850180</t>
+          <t>10636651</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>30624300</t>
+          <t>"Ismail Aflou"</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
@@ -3258,17 +3258,17 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>28624723</t>
+          <t>12648101</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>"Woody Shade"</t>
+          <t>"player 198827"</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
@@ -3285,17 +3285,17 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>6010122</t>
+          <t>15755724</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>"Edward Peng"</t>
+          <t>"Last Good"</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
@@ -3312,17 +3312,17 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>9913517</t>
+          <t>28624723</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>"Kenny Chan"</t>
+          <t>"Woody Shade"</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
@@ -3339,17 +3339,17 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>52311</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>10636651</t>
+          <t>41848598</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>"Ismail Aflou"</t>
+          <t>国家一级保护沙雕</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
@@ -3359,7 +3359,7 @@
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>3224</t>
         </is>
       </c>
     </row>

</xml_diff>